<commit_message>
AL2023 versions file added
</commit_message>
<xml_diff>
--- a/src/test/java/CloudAndSystemEngineering/ShutdownBanner/Resources/BannerUrlListProd.xlsx
+++ b/src/test/java/CloudAndSystemEngineering/ShutdownBanner/Resources/BannerUrlListProd.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bucurgb/IdeaProjects/CBIIT-Test-Automation/src/test/java/CloudAndSystemEngineering/ShutdownBanner/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6121D5B1-893C-884B-ABF4-1A7E93D4DA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DD6998-2C86-774C-840E-7C8704A14553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{7D8A36FA-F3A4-A34E-8D1B-5EE26F4A67C5}"/>
+    <workbookView minimized="1" xWindow="16960" yWindow="760" windowWidth="51200" windowHeight="18880" activeTab="5" xr2:uid="{7D8A36FA-F3A4-A34E-8D1B-5EE26F4A67C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet8" sheetId="9" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet7" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet6!$A$1:$A$411</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet6!$A$1:$A$411</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="529">
   <si>
     <t>https://ldlink-qa.nci.nih.gov/?tab=home</t>
   </si>
@@ -2024,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5D782F-EEAD-5647-AA38-F4BE1C5EC33D}">
   <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2487,30 +2486,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3273050B-E83B-AB45-832B-B1D2AF058374}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>519</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017F0611-0096-294F-B542-5996FC46EAD8}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView topLeftCell="A718" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A753" sqref="A1:A753"/>
     </sheetView>
   </sheetViews>
@@ -2530,7 +2509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC72ECBA-C062-AB47-AE04-6BE6D2CC2C43}">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -2607,13 +2586,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19844647-35E1-5B4C-A550-F0AF59FB75DB}">
   <dimension ref="A1:A411"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4693,7 +4670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84041A0-A1B6-4D4A-A070-70D8D7D5E1C0}">
   <dimension ref="A1:A31"/>
   <sheetViews>

</xml_diff>